<commit_message>
Minor improvement: design load
Put design heat load into further parameters where it was in a text file
before.
</commit_message>
<xml_diff>
--- a/column_generation_tsz/further_parameters.xlsx
+++ b/column_generation_tsz/further_parameters.xlsx
@@ -1,21 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Markus\Desktop\Studium\13. Semester\repos\workspace\column_generation_tsz\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="30" windowWidth="28515" windowHeight="13350"/>
+    <workbookView xWindow="120" yWindow="30" windowWidth="28515" windowHeight="13350" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="economics" sheetId="1" r:id="rId1"/>
     <sheet name="further_parameters" sheetId="2" r:id="rId2"/>
+    <sheet name="design_heat_load" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="72">
   <si>
     <t>Fixed costs for gas metering system</t>
   </si>
@@ -213,6 +219,24 @@
   </si>
   <si>
     <t>Maximum temperature spread in the storage</t>
+  </si>
+  <si>
+    <t>House</t>
+  </si>
+  <si>
+    <t>Heat load</t>
+  </si>
+  <si>
+    <t>ADS_1</t>
+  </si>
+  <si>
+    <t>ADS_10</t>
+  </si>
+  <si>
+    <t>ADS_11</t>
+  </si>
+  <si>
+    <t>ADS_12</t>
   </si>
 </sst>
 </file>
@@ -268,9 +292,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Larissa">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -308,9 +332,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Larissa">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -345,7 +369,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -380,7 +404,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Larissa">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -556,7 +580,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
@@ -969,4 +993,59 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2">
+        <v>11000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B3">
+        <v>16000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B4">
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B5">
+        <v>15000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>